<commit_message>
SearchView에서 엔터를 누르면 consol에 Hello World!를 띄우는데는 성공함 하지만 NAVER API호출시 android.os.NetworkOnMainThreadException 발생
</commit_message>
<xml_diff>
--- a/개발일정.xlsx
+++ b/개발일정.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3suhi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Open_Source_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D275F0FD-3F9A-48B4-8B75-99FD93A1AA3A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14030" windowHeight="4110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14025" windowHeight="4110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>김현일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,13 +128,18 @@
   </si>
   <si>
     <t>자동 그래프 갱신과 푸시 통지 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAVER UI 기능 연동 시도
+실패함</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -276,7 +282,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -310,14 +316,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,28 +607,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.83203125" customWidth="1"/>
-    <col min="3" max="20" width="28.08203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.875" customWidth="1"/>
+    <col min="3" max="20" width="28.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C1" s="12" t="s">
+    <row r="1" spans="2:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:20" ht="10" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:20" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="2:20" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:20" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -676,15 +685,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:20" ht="62" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:20" ht="62.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -699,7 +710,7 @@
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="2:20" ht="62" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:20" ht="62.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -722,7 +733,7 @@
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
     </row>
-    <row r="6" spans="2:20" ht="62" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:20" ht="62.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
@@ -745,7 +756,7 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
@@ -804,73 +815,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11" t="s">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
엑셀 수정 AsyncTask로  NetworkOnMainThreadException를 해결할 예정
</commit_message>
<xml_diff>
--- a/개발일정.xlsx
+++ b/개발일정.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Open_Source_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5C6324DA-2458-465B-9C83-369A913CACC9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{99DDDBF3-8D07-45C2-BBC5-2B6DA4F8DCA9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14025" windowHeight="4110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>김현일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -134,6 +134,11 @@
     <t>NAVER UI 기능 연동 시도
 HelloWorld는 출력했으나
 NetworkOnMainThreadException 로 인해 API호출 실패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AsyncTask로
+NetworkOnMainThreadException 처리할 것</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -612,7 +617,7 @@
   <dimension ref="B1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -693,7 +698,9 @@
       <c r="C4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="12"/>

</xml_diff>